<commit_message>
V3.0.1.14 - Mod Update
Due to recent update with MultiMC, modpack was broken. Updating Forge
and LiteLoader appears to have fixed the issue.

Updated Mods:
- Forge: 10.13.0.1182
- LiteLoader: 1.7.10_02
</commit_message>
<xml_diff>
--- a/Mod List.xlsx
+++ b/Mod List.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$207</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$236</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="283">
   <si>
     <t>Mod Name</t>
   </si>
@@ -240,9 +240,6 @@
     <t>StatusEffectHUD</t>
   </si>
   <si>
-    <t>Damage Indicators</t>
-  </si>
-  <si>
     <t>Industrial Craft 2 Experimental</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>Forestry</t>
   </si>
   <si>
-    <t>Gregtech</t>
-  </si>
-  <si>
     <t>Witchery</t>
   </si>
   <si>
@@ -726,9 +720,6 @@
     <t>1.5.6</t>
   </si>
   <si>
-    <t>Mystcraft addon</t>
-  </si>
-  <si>
     <t>Journey Map</t>
   </si>
   <si>
@@ -754,6 +745,129 @@
   </si>
   <si>
     <t>1.1.8a</t>
+  </si>
+  <si>
+    <t>1.0.0.2</t>
+  </si>
+  <si>
+    <t>Adds shortcut wheel, accessed by holding "R"</t>
+  </si>
+  <si>
+    <t>Progressive Automation</t>
+  </si>
+  <si>
+    <t>Airship Mod</t>
+  </si>
+  <si>
+    <t>Better Foliage</t>
+  </si>
+  <si>
+    <t>Void</t>
+  </si>
+  <si>
+    <t>Nearby Mob Finder</t>
+  </si>
+  <si>
+    <t>Tabula Rasa</t>
+  </si>
+  <si>
+    <t>Ore Berries</t>
+  </si>
+  <si>
+    <t>Female Gender Option</t>
+  </si>
+  <si>
+    <t>Devine RPG</t>
+  </si>
+  <si>
+    <t>MineTweaker 3</t>
+  </si>
+  <si>
+    <t>GregTech</t>
+  </si>
+  <si>
+    <t>Fabricators</t>
+  </si>
+  <si>
+    <t>Ars Magica</t>
+  </si>
+  <si>
+    <t>Alchemical Bling</t>
+  </si>
+  <si>
+    <t>Too Much Rain</t>
+  </si>
+  <si>
+    <t>ZZZZZ Custom Configs</t>
+  </si>
+  <si>
+    <t>Lockdown</t>
+  </si>
+  <si>
+    <t>Description Tags</t>
+  </si>
+  <si>
+    <t>Automagy</t>
+  </si>
+  <si>
+    <t>Noggscraft Emerald Tool and Armor</t>
+  </si>
+  <si>
+    <t>NedoComputers</t>
+  </si>
+  <si>
+    <t>Cybernetica</t>
+  </si>
+  <si>
+    <t>RC Mod</t>
+  </si>
+  <si>
+    <t>AE2 Tech Add-On Mod</t>
+  </si>
+  <si>
+    <t>Will not be included</t>
+  </si>
+  <si>
+    <t>3.0.1</t>
+  </si>
+  <si>
+    <t>1.57-116</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>Damage Indicators Mod</t>
+  </si>
+  <si>
+    <t>3.2.0</t>
+  </si>
+  <si>
+    <t>Mystcraft addon, pending 1.7.10 version</t>
+  </si>
+  <si>
+    <t>Baubles Princess Edition</t>
+  </si>
+  <si>
+    <t>Santa's Décor</t>
+  </si>
+  <si>
+    <t>ItemSearch</t>
+  </si>
+  <si>
+    <t>Statues Mod</t>
+  </si>
+  <si>
+    <t>Archimedes Ships</t>
+  </si>
+  <si>
+    <t>Flaxbeard's Steam Power</t>
+  </si>
+  <si>
+    <t>3D Furnace</t>
   </si>
 </sst>
 </file>
@@ -1104,13 +1218,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D212"/>
+  <dimension ref="A1:D242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B127" sqref="B127"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,126 +1242,129 @@
         <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>131</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>48</v>
+      <c r="C4" s="2" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>109</v>
+        <v>151</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D7" t="s">
-        <v>239</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>177</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>229</v>
+      <c r="C14" s="2">
+        <v>1.27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>77</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>4</v>
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>5</v>
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,104 +1375,104 @@
         <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>164</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>50</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>118</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>220</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>101</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>180</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>132</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>183</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>151</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>70</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6.13</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,1021 +1480,1242 @@
         <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="D39" t="s">
-        <v>232</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B45" t="s">
-        <v>190</v>
+        <v>61</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D48" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>129</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>273</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>202</v>
-      </c>
-      <c r="D54" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>59</v>
-      </c>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>98</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>188</v>
+        <v>200</v>
+      </c>
+      <c r="D66" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>119</v>
-      </c>
-      <c r="D68" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>135</v>
-      </c>
-      <c r="D69" t="s">
-        <v>232</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" t="s">
-        <v>232</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B71" t="s">
-        <v>14</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="D73" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>207</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B76" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>114</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>154</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B80" t="s">
+        <v>117</v>
+      </c>
+      <c r="D80" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>133</v>
+      </c>
+      <c r="D81" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>139</v>
+      </c>
+      <c r="D82" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B83" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>251</v>
+      </c>
+      <c r="D90" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B95" t="s">
         <v>55</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+      <c r="C95" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>221</v>
-      </c>
-      <c r="D95" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B105" t="s">
-        <v>74</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>57</v>
-      </c>
-      <c r="D109" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="D110" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>195</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B115" t="s">
-        <v>63</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>161</v>
+        <v>202</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>198</v>
+        <v>150</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>21</v>
+        <v>195</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B119" t="s">
-        <v>240</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D119" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B120" t="s">
-        <v>22</v>
+        <v>73</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>128</v>
+        <v>18</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B122" t="s">
-        <v>144</v>
+        <v>19</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>97</v>
+        <v>278</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>212</v>
+        <v>57</v>
+      </c>
+      <c r="D125" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>237</v>
+        <v>123</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>64</v>
-      </c>
-      <c r="D128" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>88</v>
+        <v>224</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B131" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>139</v>
+        <v>260</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B136" t="s">
-        <v>24</v>
+        <v>237</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D136" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B137" t="s">
-        <v>58</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>171</v>
+        <v>22</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B139" t="s">
-        <v>26</v>
-      </c>
-      <c r="C139" s="2">
-        <v>0.6</v>
+        <v>142</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>66</v>
-      </c>
-      <c r="D141" t="s">
-        <v>232</v>
+        <v>95</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="B142" t="s">
-        <v>136</v>
+        <v>210</v>
+      </c>
+      <c r="D142" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B144" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D144" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="D146" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>82</v>
+      </c>
+      <c r="D151" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D156" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B158" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B160" t="s">
-        <v>227</v>
+        <v>26</v>
+      </c>
+      <c r="C160" s="2">
+        <v>0.6</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>102</v>
-      </c>
-      <c r="D161" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>121</v>
+        <v>66</v>
+      </c>
+      <c r="D162" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>100</v>
-      </c>
-      <c r="D164" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>163</v>
+        <v>28</v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>146</v>
+        <v>29</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>36</v>
+        <v>187</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>205</v>
+        <v>141</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>37</v>
+        <v>212</v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>192</v>
+        <v>31</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>77</v>
+        <v>244</v>
       </c>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>181</v>
+        <v>113</v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>223</v>
+        <v>88</v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>140</v>
+        <v>32</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>210</v>
+        <v>33</v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>87</v>
+        <v>266</v>
       </c>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>38</v>
+        <v>185</v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>145</v>
+        <v>225</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>122</v>
+        <v>100</v>
+      </c>
+      <c r="D185" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>42</v>
+        <v>98</v>
+      </c>
+      <c r="D188" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>158</v>
-      </c>
-      <c r="D190" t="s">
-        <v>232</v>
+        <v>161</v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>225</v>
+        <v>144</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B204" t="s">
+        <v>72</v>
+      </c>
+      <c r="C204" s="2">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>156</v>
+      </c>
+      <c r="D217" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
-        <v>91</v>
-      </c>
-      <c r="D193" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B194" t="s">
-        <v>120</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B195" t="s">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>89</v>
+      </c>
+      <c r="D220" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B221" t="s">
+        <v>118</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B222" t="s">
         <v>39</v>
       </c>
-      <c r="C195" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
+      <c r="C222" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
         <v>40</v>
       </c>
-      <c r="D196" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>137</v>
-      </c>
-      <c r="D197" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
+      <c r="D223" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
+        <v>135</v>
+      </c>
+      <c r="D224" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B202" t="s">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B231" t="s">
+        <v>45</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B233" t="s">
+        <v>197</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B235" t="s">
+        <v>46</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B236" t="s">
+        <v>47</v>
+      </c>
+      <c r="D236" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B238" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B203" t="s">
-        <v>45</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B205" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
-        <v>46</v>
-      </c>
-      <c r="C206" s="3"/>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B207" t="s">
-        <v>47</v>
-      </c>
-      <c r="D207" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B208" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>259</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B207">
+  <autoFilter ref="A1:B236">
     <sortState ref="A2:B150">
       <sortCondition ref="B1:B146"/>
     </sortState>

</xml_diff>

<commit_message>
V3.0.1.15 - Stage 13 Mod Installation & Update
Newly installed mods:
- JABBA: 1.1.4
- RPG Advanced Mod: 1.0.0
- WAILA: 1.5.3

Updated Mod:
- Forge: 10.13.0.1188

Notes:
- Mod List.xlsx has now been updated. Any mods with an "X" means it has
been installed in the modpack. Any mods with a "P" means that I will be
prioritising focus on those mods, and will hopefully install those mods
ASAP once ported to 1.7.10. Any mods with a "-" means that the mod under
that name no longer should exist. Check the Extra column for more info.
</commit_message>
<xml_diff>
--- a/Mod List.xlsx
+++ b/Mod List.xlsx
@@ -12,14 +12,15 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$236</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$265</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="313">
   <si>
     <t>Mod Name</t>
   </si>
@@ -456,9 +457,6 @@
     <t>Resonant Induction</t>
   </si>
   <si>
-    <t>ICBM</t>
-  </si>
-  <si>
     <t>Tubes</t>
   </si>
   <si>
@@ -534,9 +532,6 @@
     <t>1.7.10_01</t>
   </si>
   <si>
-    <t>10.13.0.1180</t>
-  </si>
-  <si>
     <t>1.0.2.6</t>
   </si>
   <si>
@@ -868,6 +863,102 @@
   </si>
   <si>
     <t>3D Furnace</t>
+  </si>
+  <si>
+    <t>Enchvil</t>
+  </si>
+  <si>
+    <t>InvWorks</t>
+  </si>
+  <si>
+    <t>TechnoMagi</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Rock Digger</t>
+  </si>
+  <si>
+    <t>ChatFlow</t>
+  </si>
+  <si>
+    <t>Draconic Evolution</t>
+  </si>
+  <si>
+    <t>Universal Electricity</t>
+  </si>
+  <si>
+    <t>Warp Book</t>
+  </si>
+  <si>
+    <t>QuarryPlus</t>
+  </si>
+  <si>
+    <t>GrowthCraft</t>
+  </si>
+  <si>
+    <t>Morph</t>
+  </si>
+  <si>
+    <t>Computronics</t>
+  </si>
+  <si>
+    <t>HungerOverhaul</t>
+  </si>
+  <si>
+    <t>Bdew's Mods</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>RPG Advanced Mod</t>
+  </si>
+  <si>
+    <t>Modular Machines</t>
+  </si>
+  <si>
+    <t>Extra Carts</t>
+  </si>
+  <si>
+    <t>Currently in Alpha</t>
+  </si>
+  <si>
+    <t>Ported</t>
+  </si>
+  <si>
+    <t>Xycraft</t>
+  </si>
+  <si>
+    <t>Pam's Mods</t>
+  </si>
+  <si>
+    <t>Player Beacons</t>
+  </si>
+  <si>
+    <t>Hydraulicraft</t>
+  </si>
+  <si>
+    <t>Artillects</t>
+  </si>
+  <si>
+    <t>Formally ICBM</t>
+  </si>
+  <si>
+    <t>WorldEditCUI</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>1.5.3</t>
+  </si>
+  <si>
+    <t>10.13.0.1188</t>
   </si>
 </sst>
 </file>
@@ -1218,13 +1309,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D242"/>
+  <dimension ref="A1:D265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1338,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1263,7 +1354,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,11 +1363,14 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,17 +1380,17 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1307,10 +1401,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1321,12 +1415,12 @@
         <v>49</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1348,15 +1442,18 @@
         <v>77</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="B16" t="s">
         <v>104</v>
       </c>
       <c r="D16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1364,7 +1461,7 @@
         <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1375,22 +1472,22 @@
         <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,537 +1507,579 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>174</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B32" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C37" s="2">
         <v>6.13</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="C38" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B39" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>7</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>108</v>
+      </c>
+      <c r="D41" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>167</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B50" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B51" t="s">
         <v>54</v>
       </c>
-      <c r="D48" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="D51" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B52" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" t="s">
-        <v>273</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" t="s">
-        <v>158</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" t="s">
         <v>127</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>214</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>80</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>200</v>
-      </c>
-      <c r="D66" t="s">
-        <v>275</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>10</v>
+        <v>287</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>191</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>192</v>
+        <v>198</v>
+      </c>
+      <c r="D71" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>217</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" t="s">
-        <v>93</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B76" t="s">
-        <v>96</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>13</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>186</v>
+        <v>11</v>
+      </c>
+      <c r="D78" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>201</v>
+        <v>281</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="B80" t="s">
-        <v>117</v>
-      </c>
-      <c r="D80" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="B81" t="s">
-        <v>133</v>
-      </c>
-      <c r="D81" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B82" t="s">
-        <v>139</v>
-      </c>
-      <c r="D82" t="s">
-        <v>230</v>
+        <v>96</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B83" t="s">
-        <v>14</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>15</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>205</v>
+        <v>117</v>
+      </c>
+      <c r="D86" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>198</v>
+        <v>133</v>
+      </c>
+      <c r="D87" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>255</v>
+        <v>139</v>
+      </c>
+      <c r="D88" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>90</v>
+        <v>299</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B90" t="s">
-        <v>251</v>
-      </c>
-      <c r="D90" t="s">
-        <v>230</v>
+        <v>14</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>281</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="B92" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>112</v>
+        <v>203</v>
+      </c>
+      <c r="D93" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B95" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>249</v>
+      </c>
+      <c r="D97" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B100" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B102" t="s">
         <v>55</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
+      <c r="C102" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B103" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>219</v>
-      </c>
-      <c r="D110" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>216</v>
+        <v>162</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>17</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -1950,774 +2089,940 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>145</v>
+        <v>291</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>202</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>195</v>
+        <v>217</v>
+      </c>
+      <c r="D118" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>226</v>
+        <v>110</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B120" t="s">
-        <v>73</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B122" t="s">
-        <v>19</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>20</v>
+        <v>305</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>278</v>
+        <v>202</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="B125" t="s">
-        <v>57</v>
+        <v>306</v>
       </c>
       <c r="D125" t="s">
-        <v>230</v>
+        <v>307</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B130" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B132" t="s">
+        <v>19</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B136" t="s">
+        <v>57</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B142" t="s">
         <v>63</v>
       </c>
-      <c r="C131" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B136" t="s">
-        <v>237</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D136" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B142" t="s">
-        <v>210</v>
-      </c>
-      <c r="D142" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C142" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>234</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D144" t="s">
-        <v>243</v>
+        <v>158</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>253</v>
+        <v>194</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>64</v>
-      </c>
-      <c r="D146" t="s">
-        <v>230</v>
+        <v>21</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B147" t="s">
-        <v>183</v>
+        <v>235</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D147" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>82</v>
-      </c>
-      <c r="D151" t="s">
-        <v>230</v>
+        <v>91</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="B153" t="s">
-        <v>23</v>
+        <v>208</v>
+      </c>
+      <c r="D153" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>248</v>
+        <v>94</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B155" t="s">
-        <v>264</v>
+        <v>232</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D155" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>24</v>
-      </c>
-      <c r="D156" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>263</v>
+        <v>64</v>
+      </c>
+      <c r="D157" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B158" t="s">
-        <v>58</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B164" t="s">
+        <v>82</v>
+      </c>
+      <c r="D164" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B166" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>24</v>
+      </c>
+      <c r="D169" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B171" t="s">
+        <v>58</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B160" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B173" t="s">
         <v>26</v>
       </c>
-      <c r="C160" s="2">
+      <c r="C173" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B175" t="s">
         <v>66</v>
       </c>
-      <c r="D162" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
+      <c r="D175" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B166" t="s">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B167" t="s">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B169" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B177" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B193" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B195" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B197" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
         <v>100</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D201" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B186" t="s">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B187" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
         <v>98</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D204" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B189" t="s">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B190" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B191" t="s">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B192" t="s">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B194" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B195" t="s">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B212" t="s">
+        <v>297</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B202" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B204" t="s">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B222" t="s">
         <v>72</v>
       </c>
-      <c r="C204" s="2">
+      <c r="C222" s="2">
         <v>1.26</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B205" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B207" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B208" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B215" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B217" t="s">
-        <v>156</v>
-      </c>
-      <c r="D217" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B219" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
-        <v>89</v>
-      </c>
-      <c r="D220" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B221" t="s">
-        <v>118</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B222" t="s">
-        <v>39</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
-        <v>40</v>
-      </c>
-      <c r="D223" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B224" t="s">
-        <v>135</v>
-      </c>
-      <c r="D224" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="B226" t="s">
-        <v>258</v>
+        <v>85</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>44</v>
+        <v>247</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>146</v>
+        <v>283</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B231" t="s">
-        <v>45</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>220</v>
+        <v>120</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="B232" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B233" t="s">
-        <v>197</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>272</v>
+        <v>41</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>247</v>
+        <v>42</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B235" t="s">
-        <v>46</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>271</v>
+        <v>122</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>47</v>
+        <v>155</v>
       </c>
       <c r="D236" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>131</v>
+        <v>221</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>211</v>
+        <v>89</v>
+      </c>
+      <c r="D239" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B241" t="s">
+        <v>118</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B242" t="s">
+        <v>39</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>40</v>
+      </c>
+      <c r="D243" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B244" t="s">
+        <v>135</v>
+      </c>
+      <c r="D244" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B245" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B248" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B250" t="s">
+        <v>45</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B251" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B253" t="s">
+        <v>195</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B254" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B255" t="s">
+        <v>46</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B256" t="s">
+        <v>47</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B257" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B258" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B259" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B260" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B261" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B241" t="s">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B262" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B263" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B242" t="s">
-        <v>259</v>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B264" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B265" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B236">
-    <sortState ref="A2:B150">
-      <sortCondition ref="B1:B146"/>
+  <autoFilter ref="A1:D265">
+    <sortState ref="A2:D257">
+      <sortCondition ref="B1:B257"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
V3.0.1.19 - Stage 17 Mod Installation
Newly installed mod:
- Ender IO: 2.0 beta.147

Note:
- New configs have not been fully checked as of this commit. Please
check configs at a later date.
</commit_message>
<xml_diff>
--- a/Mod List.xlsx
+++ b/Mod List.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$266</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$274</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="329">
   <si>
     <t>Mod Name</t>
   </si>
@@ -1004,6 +1004,9 @@
   </si>
   <si>
     <t>Mouse Tweaks</t>
+  </si>
+  <si>
+    <t>Not Enough Keys</t>
   </si>
 </sst>
 </file>
@@ -1354,13 +1357,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F273"/>
+  <dimension ref="A1:F274"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B269" sqref="B269"/>
+      <selection pane="bottomRight" activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,414 +2604,408 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B180" t="s">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B181" t="s">
         <v>26</v>
       </c>
-      <c r="C180" s="2">
+      <c r="C181" s="2">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B184" t="s">
         <v>66</v>
       </c>
-      <c r="F183" t="s">
+      <c r="F184" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>134</v>
+        <v>246</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>301</v>
+        <v>28</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>29</v>
+        <v>301</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>185</v>
+        <v>30</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>128</v>
+        <v>210</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>302</v>
+        <v>128</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>31</v>
+        <v>302</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>213</v>
+        <v>31</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B202" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B202" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B204" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="1" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B206" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>183</v>
+        <v>262</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>100</v>
-      </c>
-      <c r="F209" t="s">
-        <v>102</v>
+        <v>223</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>119</v>
+        <v>100</v>
+      </c>
+      <c r="F210" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>98</v>
-      </c>
-      <c r="F212" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>34</v>
+        <v>98</v>
+      </c>
+      <c r="F213" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>160</v>
+        <v>34</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>283</v>
+        <v>144</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>35</v>
+        <v>283</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B220" t="s">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B221" t="s">
         <v>295</v>
       </c>
-      <c r="C220" s="2" t="s">
+      <c r="C221" s="2" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B221" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>273</v>
+        <v>37</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>132</v>
+        <v>273</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>188</v>
+        <v>132</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B230" t="s">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B231" t="s">
         <v>72</v>
       </c>
-      <c r="C230" s="2">
+      <c r="C231" s="2">
         <v>1.26</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B231" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B235" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B235" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>38</v>
+        <v>245</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>281</v>
+        <v>38</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>143</v>
+        <v>281</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B241" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B241" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>155</v>
-      </c>
-      <c r="F244" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>221</v>
+        <v>155</v>
+      </c>
+      <c r="F245" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>43</v>
+        <v>221</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>89</v>
-      </c>
-      <c r="F247" t="s">
-        <v>228</v>
+        <v>43</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
+        <v>89</v>
+      </c>
+      <c r="F248" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B249" t="s">
-        <v>118</v>
-      </c>
-      <c r="C249" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
@@ -3016,167 +3013,178 @@
         <v>59</v>
       </c>
       <c r="B250" t="s">
+        <v>118</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B251" t="s">
         <v>39</v>
       </c>
-      <c r="C250" s="2" t="s">
+      <c r="C251" s="2" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B251" t="s">
-        <v>40</v>
-      </c>
-      <c r="F251" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="F252" t="s">
-        <v>228</v>
+        <v>299</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>254</v>
+        <v>135</v>
+      </c>
+      <c r="F253" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>182</v>
+        <v>254</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>44</v>
+        <v>182</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B258" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B258" t="s">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B259" t="s">
         <v>45</v>
       </c>
-      <c r="C258" s="2" t="s">
+      <c r="C259" s="2" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B259" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B261" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B261" t="s">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B262" t="s">
         <v>195</v>
       </c>
-      <c r="C261" s="2" t="s">
+      <c r="C262" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B262" t="s">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B263" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B263" t="s">
-        <v>46</v>
-      </c>
-      <c r="C263" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D263" s="3"/>
-      <c r="E263" s="3"/>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B264" t="s">
+        <v>46</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D264" s="3"/>
+      <c r="E264" s="3"/>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B265" t="s">
         <v>47</v>
       </c>
-      <c r="C264" s="2" t="s">
+      <c r="C265" s="2" t="s">
         <v>309</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B265" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B267" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A267" s="1" t="s">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B267" t="s">
+      <c r="B268" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B268" t="s">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B269" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B269" t="s">
+      <c r="B270" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B270" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>65</v>
+        <v>306</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>300</v>
+        <v>65</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
         <v>255</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F266">
+  <autoFilter ref="A1:F274">
     <sortState ref="A2:F273">
       <sortCondition ref="B1:B266"/>
     </sortState>

</xml_diff>

<commit_message>
V3.0.1.20 - Stage 18 Mod Installation
Newly installed mods:
- Ender Utilities: 0.2.0
- Extra Utilities: 1.1.0e

Updated mod:
- Forge: 10.13.0.1199

Note:
- New config has not been checked. Please check at a later date.
</commit_message>
<xml_diff>
--- a/Mod List.xlsx
+++ b/Mod List.xlsx
@@ -12,15 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$274</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$275</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="348">
   <si>
     <t>Mod Name</t>
   </si>
@@ -256,9 +255,6 @@
     <t>Aroma1997Core</t>
   </si>
   <si>
-    <t>Biomes o' Plenty</t>
-  </si>
-  <si>
     <t>CustomMobSpawner</t>
   </si>
   <si>
@@ -952,9 +948,6 @@
     <t>1.5.3</t>
   </si>
   <si>
-    <t>10.13.0.1188</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -1007,6 +1000,69 @@
   </si>
   <si>
     <t>Not Enough Keys</t>
+  </si>
+  <si>
+    <t>Thermal Foundation</t>
+  </si>
+  <si>
+    <t>FLORA</t>
+  </si>
+  <si>
+    <t>Torchools</t>
+  </si>
+  <si>
+    <t>IHL Tools &amp; Machines</t>
+  </si>
+  <si>
+    <t>Races for Minecraft</t>
+  </si>
+  <si>
+    <t>Craft Heraldry</t>
+  </si>
+  <si>
+    <t>Builder's Guides</t>
+  </si>
+  <si>
+    <t>Spatial IO Compat</t>
+  </si>
+  <si>
+    <t>MoarPeripherals</t>
+  </si>
+  <si>
+    <t>Deepcore</t>
+  </si>
+  <si>
+    <t>Quick Hotbar Mod</t>
+  </si>
+  <si>
+    <t>LanteaCraft</t>
+  </si>
+  <si>
+    <t>2.0 beta.147</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>BiblioWoods Biomes O'Plenty Edition</t>
+  </si>
+  <si>
+    <t>Biomes O' Plenty</t>
+  </si>
+  <si>
+    <t>1.7.4</t>
+  </si>
+  <si>
+    <t>1.0.2.16</t>
+  </si>
+  <si>
+    <t>10.13.0.1199</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>1.1.0e</t>
   </si>
 </sst>
 </file>
@@ -1357,13 +1413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F274"/>
+  <dimension ref="A1:F287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B180" sqref="B180"/>
+      <selection pane="bottomRight" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,10 +1437,10 @@
         <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F1" t="s">
         <v>74</v>
@@ -1392,12 +1448,12 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1408,13 +1464,13 @@
         <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1424,41 +1480,41 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1469,13 +1525,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F12" t="s">
         <v>313</v>
-      </c>
-      <c r="F12" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1486,32 +1542,32 @@
         <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,7 +1581,7 @@
         <v>1.27</v>
       </c>
       <c r="F16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1536,10 +1592,10 @@
         <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1547,21 +1603,21 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>99</v>
+        <v>344</v>
       </c>
       <c r="F18" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1569,39 +1625,39 @@
         <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22" t="s">
+        <v>303</v>
+      </c>
+      <c r="F22" t="s">
         <v>304</v>
-      </c>
-      <c r="F22" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1621,22 +1677,22 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,13 +1700,13 @@
         <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F32" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1661,69 +1717,69 @@
         <v>50</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>99</v>
+        <v>343</v>
       </c>
       <c r="F33" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>341</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1.6</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" t="s">
-        <v>315</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B36" t="s">
-        <v>282</v>
+        <v>342</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F36" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B37" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>6</v>
+      <c r="C38" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F38" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>216</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="2">
-        <v>6.13</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1731,172 +1787,172 @@
         <v>59</v>
       </c>
       <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="2">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>130</v>
+      <c r="C42" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="B44" t="s">
-        <v>108</v>
-      </c>
-      <c r="F44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>7</v>
+        <v>107</v>
+      </c>
+      <c r="F45" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>179</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>284</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>148</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>294</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>61</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B53" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
-      </c>
-      <c r="F54" t="s">
-        <v>228</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B56" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>178</v>
+        <v>290</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B60" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B61" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>186</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" t="s">
+        <v>268</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B65" t="s">
-        <v>157</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>265</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1904,112 +1960,118 @@
         <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>175</v>
+        <v>264</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B67" t="s">
-        <v>257</v>
+        <v>126</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>87</v>
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>212</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>285</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>80</v>
+        <v>284</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>198</v>
-      </c>
-      <c r="F74" t="s">
-        <v>271</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>109</v>
+        <v>197</v>
+      </c>
+      <c r="F75" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>205</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" t="s">
-        <v>93</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>279</v>
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>294</v>
+        <v>59</v>
       </c>
       <c r="B84" t="s">
-        <v>211</v>
+        <v>12</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2017,1006 +2079,1009 @@
         <v>59</v>
       </c>
       <c r="B85" t="s">
-        <v>96</v>
+        <v>210</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>167</v>
+        <v>346</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B86" t="s">
-        <v>13</v>
+        <v>95</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>184</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>117</v>
-      </c>
-      <c r="F89" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="F90" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F91" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>297</v>
+        <v>138</v>
+      </c>
+      <c r="F92" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B93" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B94" t="s">
         <v>14</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>197</v>
+      <c r="C94" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B95" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B96" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>203</v>
-      </c>
-      <c r="F96" t="s">
-        <v>298</v>
+      <c r="C96" s="2" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>196</v>
+        <v>202</v>
+      </c>
+      <c r="F97" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>251</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B99" t="s">
-        <v>90</v>
+        <v>250</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="B100" t="s">
-        <v>247</v>
-      </c>
-      <c r="F100" t="s">
-        <v>228</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>277</v>
+        <v>246</v>
+      </c>
+      <c r="F101" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>151</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B103" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="B104" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B105" t="s">
-        <v>55</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>310</v>
+        <v>111</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>294</v>
+        <v>59</v>
       </c>
       <c r="B106" t="s">
+        <v>55</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B107" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>220</v>
+        <v>62</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>125</v>
+        <v>225</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>154</v>
+        <v>226</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>250</v>
+        <v>161</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>204</v>
+        <v>249</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>289</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>16</v>
+        <v>288</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>217</v>
-      </c>
-      <c r="F121" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>110</v>
+        <v>216</v>
+      </c>
+      <c r="F122" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>324</v>
+        <v>109</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>214</v>
+        <v>322</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>17</v>
+        <v>213</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>292</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>202</v>
+        <v>302</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>149</v>
+        <v>199</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B133" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B134" t="s">
         <v>73</v>
       </c>
-      <c r="C133" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
+      <c r="C134" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B135" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B136" t="s">
         <v>19</v>
       </c>
-      <c r="C135" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>280</v>
+      <c r="C136" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>20</v>
+        <v>279</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>274</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B139" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B140" t="s">
         <v>57</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
-        <v>180</v>
+      <c r="C140" s="2" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>123</v>
+        <v>179</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>230</v>
+        <v>122</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>191</v>
+        <v>229</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B145" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B146" t="s">
         <v>63</v>
       </c>
-      <c r="C145" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
-        <v>256</v>
+      <c r="C146" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>158</v>
+        <v>255</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B150" t="s">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B151" t="s">
+        <v>232</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="F151" t="s">
         <v>234</v>
-      </c>
-      <c r="F150" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B151" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>323</v>
+        <v>22</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>126</v>
+        <v>321</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>326</v>
+        <v>90</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>95</v>
+        <v>324</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="B158" t="s">
-        <v>208</v>
-      </c>
-      <c r="F158" t="s">
-        <v>264</v>
+        <v>94</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="B159" t="s">
-        <v>94</v>
+        <v>207</v>
+      </c>
+      <c r="F159" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B160" t="s">
-        <v>320</v>
+        <v>93</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>59</v>
+        <v>293</v>
       </c>
       <c r="B161" t="s">
-        <v>231</v>
-      </c>
-      <c r="C161" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B162" t="s">
+        <v>230</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F162" t="s">
         <v>238</v>
-      </c>
-      <c r="F161" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>64</v>
-      </c>
-      <c r="F163" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>181</v>
+        <v>64</v>
+      </c>
+      <c r="F164" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>86</v>
+        <v>180</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>296</v>
+        <v>85</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>136</v>
+        <v>295</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>290</v>
+        <v>136</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B171" t="s">
-        <v>82</v>
-      </c>
-      <c r="F171" t="s">
-        <v>228</v>
+        <v>325</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="B172" t="s">
-        <v>187</v>
+        <v>81</v>
+      </c>
+      <c r="F172" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B173" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B174" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>24</v>
-      </c>
-      <c r="F176" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>259</v>
+        <v>24</v>
+      </c>
+      <c r="F177" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B178" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B179" t="s">
         <v>58</v>
       </c>
-      <c r="C178" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>328</v>
+      <c r="C179" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B181" t="s">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B182" t="s">
         <v>26</v>
       </c>
-      <c r="C181" s="2">
+      <c r="C182" s="2">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>325</v>
+        <v>152</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B184" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B185" t="s">
         <v>66</v>
       </c>
-      <c r="F184" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
-        <v>246</v>
+      <c r="F185" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>134</v>
+        <v>245</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>301</v>
+        <v>28</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>29</v>
+        <v>300</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>185</v>
+        <v>30</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>141</v>
+        <v>184</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>128</v>
+        <v>209</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>302</v>
+        <v>127</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>31</v>
+        <v>301</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>213</v>
+        <v>31</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>240</v>
+        <v>191</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>113</v>
+        <v>239</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B202" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="B203" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B204" t="s">
-        <v>288</v>
+        <v>87</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="B205" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B206" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B207" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B207" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>183</v>
+        <v>261</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>223</v>
+        <v>182</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>100</v>
-      </c>
-      <c r="F210" t="s">
-        <v>102</v>
+        <v>222</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>119</v>
+        <v>99</v>
+      </c>
+      <c r="F211" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>98</v>
-      </c>
-      <c r="F213" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>34</v>
+        <v>97</v>
+      </c>
+      <c r="F214" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>160</v>
+        <v>34</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>283</v>
+        <v>143</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>35</v>
+        <v>282</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>201</v>
+        <v>36</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B221" t="s">
-        <v>295</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>308</v>
+        <v>200</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B222" t="s">
-        <v>37</v>
+        <v>294</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>273</v>
+        <v>37</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>132</v>
+        <v>272</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>188</v>
+        <v>131</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>97</v>
+        <v>158</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>275</v>
+        <v>176</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B231" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B232" t="s">
         <v>72</v>
       </c>
-      <c r="C231" s="2">
+      <c r="C232" s="2">
         <v>1.26</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B232" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>206</v>
+        <v>137</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B235" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="B236" t="s">
-        <v>245</v>
+        <v>84</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>38</v>
+        <v>244</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>281</v>
+        <v>38</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>143</v>
+        <v>280</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B242" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B241" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B242" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>155</v>
-      </c>
-      <c r="F245" t="s">
-        <v>228</v>
+        <v>121</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>221</v>
+        <v>154</v>
+      </c>
+      <c r="F246" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>43</v>
+        <v>220</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>89</v>
-      </c>
-      <c r="F248" t="s">
-        <v>228</v>
+        <v>43</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>207</v>
+        <v>88</v>
+      </c>
+      <c r="F249" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B250" t="s">
-        <v>118</v>
-      </c>
-      <c r="C250" s="2" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
@@ -3024,167 +3089,238 @@
         <v>59</v>
       </c>
       <c r="B251" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B252" t="s">
-        <v>40</v>
-      </c>
-      <c r="F252" t="s">
-        <v>299</v>
+        <v>39</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="F253" t="s">
-        <v>228</v>
+        <v>298</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>254</v>
+        <v>134</v>
+      </c>
+      <c r="F254" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>182</v>
+        <v>253</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>44</v>
+        <v>181</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B259" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B260" t="s">
         <v>45</v>
       </c>
-      <c r="C259" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B260" t="s">
-        <v>286</v>
+      <c r="C260" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>156</v>
+        <v>285</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B262" t="s">
-        <v>195</v>
-      </c>
-      <c r="C262" s="2" t="s">
-        <v>268</v>
+        <v>155</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B263" t="s">
-        <v>243</v>
+        <v>194</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B264" t="s">
-        <v>46</v>
-      </c>
-      <c r="C264" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D264" s="3"/>
-      <c r="E264" s="3"/>
+        <v>242</v>
+      </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B265" t="s">
+        <v>46</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D265" s="3"/>
+      <c r="E265" s="3"/>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B266" t="s">
         <v>47</v>
       </c>
-      <c r="C265" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B266" t="s">
-        <v>131</v>
+      <c r="C266" s="2" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>287</v>
+        <v>130</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A268" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B268" t="s">
-        <v>84</v>
+        <v>286</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="B269" t="s">
-        <v>209</v>
+        <v>83</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A270" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B270" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B271" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B271" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>65</v>
+        <v>305</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
-        <v>300</v>
+        <v>65</v>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>255</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B275" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B276" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B278" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B279" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B280" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B281" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B282" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B283" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B284" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B285" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B287" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F274">
+  <autoFilter ref="A1:F275">
     <sortState ref="A2:F273">
       <sortCondition ref="B1:B266"/>
     </sortState>

</xml_diff>

<commit_message>
V3.0.1.22 - Stage 20 Mod Installation
Newly installed mods:
- Iron Chest: 6.0.41.729
- Natura: 2.2.0 b1
- QuarryPlus: 1.5.7.6
- RandomThings: 2.1.2

Note:
- New configs have not been checked. Please check them at a later date.
</commit_message>
<xml_diff>
--- a/Mod List.xlsx
+++ b/Mod List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="354">
   <si>
     <t>Mod Name</t>
   </si>
@@ -1063,6 +1063,24 @@
   </si>
   <si>
     <t>1.1.0e</t>
+  </si>
+  <si>
+    <t>0.8.86</t>
+  </si>
+  <si>
+    <t>4.4.5.44</t>
+  </si>
+  <si>
+    <t>1.1.0.296</t>
+  </si>
+  <si>
+    <t>6.0.41.729</t>
+  </si>
+  <si>
+    <t>2.2.0 b1</t>
+  </si>
+  <si>
+    <t>1.5.7.6</t>
   </si>
 </sst>
 </file>
@@ -1416,10 +1434,10 @@
   <dimension ref="A1:F287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C200" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C96" sqref="C96"/>
+      <selection pane="bottomRight" activeCell="C208" sqref="C208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,10 +2205,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>293</v>
+        <v>59</v>
       </c>
       <c r="B100" t="s">
         <v>89</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,10 +2258,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>293</v>
+        <v>59</v>
       </c>
       <c r="B107" t="s">
         <v>56</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2409,8 +2433,14 @@
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B138" t="s">
         <v>20</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,10 +2668,13 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>293</v>
+        <v>59</v>
       </c>
       <c r="B174" t="s">
         <v>23</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,91 +2788,100 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>293</v>
+        <v>59</v>
       </c>
       <c r="B203" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C203" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>293</v>
+        <v>59</v>
       </c>
       <c r="B205" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C205" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>293</v>
+        <v>59</v>
       </c>
       <c r="B207" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C207" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>261</v>
       </c>

</xml_diff>

<commit_message>
Updated Modlist file (again)
</commit_message>
<xml_diff>
--- a/Mod List.xlsx
+++ b/Mod List.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="406">
   <si>
     <t>Mod Name</t>
   </si>
@@ -1233,6 +1233,9 @@
   </si>
   <si>
     <t>1.2.9 we5.6.2</t>
+  </si>
+  <si>
+    <t>1.7.10</t>
   </si>
 </sst>
 </file>
@@ -1641,10 +1644,10 @@
   <dimension ref="A1:G287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C210" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C273" sqref="C273"/>
+      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,10 +2399,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>290</v>
+        <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>68</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>405</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>387</v>

</xml_diff>